<commit_message>
trying to make autofit faster
</commit_message>
<xml_diff>
--- a/server/src/static/sexexample.xlsx
+++ b/server/src/static/sexexample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="20" windowWidth="21260" windowHeight="14060" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="21255" windowHeight="14055" tabRatio="822" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="Constants" sheetId="12" r:id="rId12"/>
     <sheet name="Economics and costs" sheetId="13" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -480,8 +480,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -646,9 +646,6 @@
     <xf numFmtId="9" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -674,6 +671,9 @@
     <xf numFmtId="10" fontId="5" fillId="5" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Input" xfId="1"/>
@@ -681,6 +681,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -968,7 +973,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:A29"/>
   <sheetViews>
@@ -976,130 +981,129 @@
       <selection sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="80.75" customWidth="1"/>
+    <col min="1" max="1" width="80.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
-      <c r="A2" s="13"/>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="13"/>
-    </row>
-    <row r="4" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="22"/>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:1" ht="65" customHeight="1">
+    <row r="5" spans="1:1" ht="65.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:1" ht="80" customHeight="1">
+    <row r="13" spans="1:1" ht="80.099999999999994" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:1" ht="57" customHeight="1">
+    <row r="19" spans="1:1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="1">
     <mergeCell ref="A1:A3"/>
   </mergeCells>
@@ -1117,7 +1121,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D25"/>
   <sheetViews>
@@ -1125,17 +1129,17 @@
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="12.75" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1145,7 +1149,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1155,7 +1159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1163,12 +1167,12 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1178,7 +1182,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1188,7 +1192,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1196,12 +1200,12 @@
       <c r="C11" s="7"/>
       <c r="D11" s="7"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1211,7 +1215,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1219,7 +1223,7 @@
       <c r="C17" s="7"/>
       <c r="D17" s="7"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1227,12 +1231,12 @@
       <c r="C18" s="7"/>
       <c r="D18" s="7"/>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1242,7 +1246,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1250,7 +1254,7 @@
       <c r="C24" s="7"/>
       <c r="D24" s="7"/>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1259,7 +1263,6 @@
       <c r="D25" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1271,23 +1274,23 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="12.75" customWidth="1"/>
+    <col min="3" max="4" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1297,7 +1300,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1305,7 +1308,7 @@
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1313,12 +1316,12 @@
       <c r="C4" s="7"/>
       <c r="D4" s="7"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C9" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1328,7 +1331,7 @@
         <v>Females 15-49</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -1336,7 +1339,7 @@
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -1345,7 +1348,6 @@
       <c r="D11" s="7"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -1357,23 +1359,25 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:E85"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="40.75" customWidth="1"/>
+    <col min="2" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C2" s="6" t="s">
         <v>85</v>
       </c>
@@ -1384,7 +1388,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
         <v>17</v>
       </c>
@@ -1398,7 +1402,7 @@
         <v>1.4E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
         <v>18</v>
       </c>
@@ -1412,7 +1416,7 @@
         <v>1.1000000000000001E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
@@ -1426,7 +1430,7 @@
         <v>1.8599999999999998E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
         <v>20</v>
       </c>
@@ -1440,7 +1444,7 @@
         <v>2.8E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="5" t="s">
         <v>21</v>
       </c>
@@ -1454,7 +1458,7 @@
         <v>2.4E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="5" t="s">
         <v>22</v>
       </c>
@@ -1468,7 +1472,7 @@
         <v>0.44</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="5" t="s">
         <v>23</v>
       </c>
@@ -1482,12 +1486,12 @@
         <v>0.27</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>85</v>
       </c>
@@ -1498,7 +1502,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="5" t="s">
         <v>25</v>
       </c>
@@ -1512,7 +1516,7 @@
         <v>48.02</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="5" t="s">
         <v>26</v>
       </c>
@@ -1526,7 +1530,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>27</v>
       </c>
@@ -1540,7 +1544,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="5" t="s">
         <v>28</v>
       </c>
@@ -1554,7 +1558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
@@ -1568,7 +1572,7 @@
         <v>6.92</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="5" t="s">
         <v>30</v>
       </c>
@@ -1582,12 +1586,12 @@
         <v>12.08</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C25" s="6" t="s">
         <v>85</v>
       </c>
@@ -1598,7 +1602,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="5" t="s">
         <v>32</v>
       </c>
@@ -1612,7 +1616,7 @@
         <v>9.76</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="5" t="s">
         <v>27</v>
       </c>
@@ -1626,7 +1630,7 @@
         <v>1.61</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="5" t="s">
         <v>33</v>
       </c>
@@ -1640,7 +1644,7 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="5" t="s">
         <v>34</v>
       </c>
@@ -1654,7 +1658,7 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="5" t="s">
         <v>35</v>
       </c>
@@ -1668,12 +1672,12 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>85</v>
       </c>
@@ -1684,7 +1688,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B36" s="5" t="s">
         <v>37</v>
       </c>
@@ -1698,7 +1702,7 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B37" s="5" t="s">
         <v>38</v>
       </c>
@@ -1712,7 +1716,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B38" s="5" t="s">
         <v>39</v>
       </c>
@@ -1726,7 +1730,7 @@
         <v>0.72</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B39" s="5" t="s">
         <v>40</v>
       </c>
@@ -1740,12 +1744,12 @@
         <v>1.96</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C44" s="6" t="s">
         <v>85</v>
       </c>
@@ -1756,7 +1760,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B45" s="5" t="s">
         <v>42</v>
       </c>
@@ -1770,7 +1774,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B46" s="5" t="s">
         <v>43</v>
       </c>
@@ -1784,12 +1788,12 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C51" s="6" t="s">
         <v>85</v>
       </c>
@@ -1800,7 +1804,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B52" s="5" t="s">
         <v>25</v>
       </c>
@@ -1814,7 +1818,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B53" s="5" t="s">
         <v>26</v>
       </c>
@@ -1828,7 +1832,7 @@
         <v>4.4000000000000003E-3</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B54" s="5" t="s">
         <v>45</v>
       </c>
@@ -1842,7 +1846,7 @@
         <v>7.1000000000000004E-3</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B55" s="5" t="s">
         <v>28</v>
       </c>
@@ -1856,7 +1860,7 @@
         <v>1.01E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B56" s="5" t="s">
         <v>29</v>
       </c>
@@ -1870,21 +1874,21 @@
         <v>7.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B57" s="5" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="8">
-        <v>0.32300000000000001</v>
+        <v>0.123</v>
       </c>
       <c r="D57" s="8">
-        <v>0.29599999999999999</v>
+        <v>0.19600000000000001</v>
       </c>
       <c r="E57" s="8">
-        <v>0.432</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
+        <v>0.23200000000000001</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B58" s="5" t="s">
         <v>46</v>
       </c>
@@ -1898,7 +1902,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B59" s="5" t="s">
         <v>47</v>
       </c>
@@ -1912,12 +1916,12 @@
         <v>3.71</v>
       </c>
     </row>
-    <row r="63" spans="1:5">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="64" spans="1:5">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C64" s="6" t="s">
         <v>85</v>
       </c>
@@ -1928,7 +1932,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="65" spans="1:5">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B65" s="5" t="s">
         <v>49</v>
       </c>
@@ -1942,7 +1946,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:5">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="5" t="s">
         <v>50</v>
       </c>
@@ -1956,7 +1960,7 @@
         <v>0.53</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="5" t="s">
         <v>51</v>
       </c>
@@ -1970,7 +1974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:5">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="5" t="s">
         <v>52</v>
       </c>
@@ -1984,7 +1988,7 @@
         <v>5.19</v>
       </c>
     </row>
-    <row r="69" spans="1:5">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="5" t="s">
         <v>53</v>
       </c>
@@ -1998,7 +2002,7 @@
         <v>1.35</v>
       </c>
     </row>
-    <row r="70" spans="1:5">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="5" t="s">
         <v>54</v>
       </c>
@@ -2012,7 +2016,7 @@
         <v>0.67</v>
       </c>
     </row>
-    <row r="71" spans="1:5">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="5" t="s">
         <v>55</v>
       </c>
@@ -2026,7 +2030,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="72" spans="1:5">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="5" t="s">
         <v>77</v>
       </c>
@@ -2040,7 +2044,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="73" spans="1:5">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="5" t="s">
         <v>56</v>
       </c>
@@ -2054,12 +2058,12 @@
         <v>0.35</v>
       </c>
     </row>
-    <row r="77" spans="1:5">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:5">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="C78" s="6" t="s">
         <v>85</v>
       </c>
@@ -2070,7 +2074,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="79" spans="1:5">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="5" t="s">
         <v>58</v>
       </c>
@@ -2084,7 +2088,7 @@
         <v>0.20499999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:5">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B80" s="5" t="s">
         <v>59</v>
       </c>
@@ -2098,7 +2102,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="81" spans="2:5">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B81" s="5" t="s">
         <v>60</v>
       </c>
@@ -2112,7 +2116,7 @@
         <v>2.9000000000000001E-2</v>
       </c>
     </row>
-    <row r="82" spans="2:5">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B82" s="5" t="s">
         <v>61</v>
       </c>
@@ -2126,7 +2130,7 @@
         <v>9.4E-2</v>
       </c>
     </row>
-    <row r="83" spans="2:5">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B83" s="5" t="s">
         <v>62</v>
       </c>
@@ -2140,7 +2144,7 @@
         <v>0.47399999999999998</v>
       </c>
     </row>
-    <row r="84" spans="2:5">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B84" s="5" t="s">
         <v>63</v>
       </c>
@@ -2154,7 +2158,7 @@
         <v>0.71499999999999997</v>
       </c>
     </row>
-    <row r="85" spans="2:5">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B85" s="5" t="s">
         <v>64</v>
       </c>
@@ -2169,7 +2173,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -2181,7 +2184,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:V91"/>
   <sheetViews>
@@ -2189,130 +2192,130 @@
       <selection sqref="A1:V91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="T1" s="17" t="s">
+      <c r="T1" s="16" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:22">
-      <c r="C2" s="17">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C2" s="16">
         <v>2000</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="16">
         <v>2001</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="16">
         <v>2002</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="16">
         <v>2003</v>
       </c>
-      <c r="G2" s="17">
+      <c r="G2" s="16">
         <v>2004</v>
       </c>
-      <c r="H2" s="17">
+      <c r="H2" s="16">
         <v>2005</v>
       </c>
-      <c r="I2" s="17">
+      <c r="I2" s="16">
         <v>2006</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="16">
         <v>2007</v>
       </c>
-      <c r="K2" s="17">
+      <c r="K2" s="16">
         <v>2008</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="16">
         <v>2009</v>
       </c>
-      <c r="M2" s="17">
+      <c r="M2" s="16">
         <v>2010</v>
       </c>
-      <c r="N2" s="17">
+      <c r="N2" s="16">
         <v>2011</v>
       </c>
-      <c r="O2" s="17">
+      <c r="O2" s="16">
         <v>2012</v>
       </c>
-      <c r="P2" s="17">
+      <c r="P2" s="16">
         <v>2013</v>
       </c>
-      <c r="Q2" s="17">
+      <c r="Q2" s="16">
         <v>2014</v>
       </c>
-      <c r="R2" s="17">
+      <c r="R2" s="16">
         <v>2015</v>
       </c>
-      <c r="T2" s="17" t="s">
+      <c r="T2" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U2" s="17" t="s">
+      <c r="U2" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V2" s="17" t="s">
+      <c r="V2" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:22">
-      <c r="B3" s="17" t="s">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="17">
         <v>75.018454192929113</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="17">
         <v>76.070810544531554</v>
       </c>
-      <c r="E3" s="18">
+      <c r="E3" s="17">
         <v>77.902335510111072</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <v>79.45534236885652</v>
       </c>
-      <c r="G3" s="18">
+      <c r="G3" s="17">
         <v>81.068347459232555</v>
       </c>
-      <c r="H3" s="18">
+      <c r="H3" s="17">
         <v>82.769770996223016</v>
       </c>
-      <c r="I3" s="18">
+      <c r="I3" s="17">
         <v>84.249516856345011</v>
       </c>
-      <c r="J3" s="18">
+      <c r="J3" s="17">
         <v>85.442534325304138</v>
       </c>
-      <c r="K3" s="18">
+      <c r="K3" s="17">
         <v>89.999873687933118</v>
       </c>
-      <c r="L3" s="18">
+      <c r="L3" s="17">
         <v>89.504730386893897</v>
       </c>
-      <c r="M3" s="18">
+      <c r="M3" s="17">
         <v>92.521062537104171</v>
       </c>
-      <c r="N3" s="18">
+      <c r="N3" s="17">
         <v>95.719284063206572</v>
       </c>
-      <c r="O3" s="18">
+      <c r="O3" s="17">
         <v>98.951609847288623</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="17">
         <v>100</v>
       </c>
-      <c r="Q3" s="18">
+      <c r="Q3" s="17">
         <f>P3*(1.025)</f>
         <v>102.49999999999999</v>
       </c>
-      <c r="R3" s="18">
+      <c r="R3" s="17">
         <f>Q3*(1.025)</f>
         <v>105.06249999999997</v>
       </c>
-      <c r="S3" s="19" t="s">
+      <c r="S3" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T3" s="12">
@@ -2325,72 +2328,72 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="7" spans="1:22">
-      <c r="A7" s="16" t="s">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:22">
-      <c r="C8" s="17">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C8" s="16">
         <v>2000</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>2001</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="16">
         <v>2002</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="16">
         <v>2003</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="16">
         <v>2004</v>
       </c>
-      <c r="H8" s="17">
+      <c r="H8" s="16">
         <v>2005</v>
       </c>
-      <c r="I8" s="17">
+      <c r="I8" s="16">
         <v>2006</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="16">
         <v>2007</v>
       </c>
-      <c r="K8" s="17">
+      <c r="K8" s="16">
         <v>2008</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="16">
         <v>2009</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>2010</v>
       </c>
-      <c r="N8" s="17">
+      <c r="N8" s="16">
         <v>2011</v>
       </c>
-      <c r="O8" s="17">
+      <c r="O8" s="16">
         <v>2012</v>
       </c>
-      <c r="P8" s="17">
+      <c r="P8" s="16">
         <v>2013</v>
       </c>
-      <c r="Q8" s="17">
+      <c r="Q8" s="16">
         <v>2014</v>
       </c>
-      <c r="R8" s="17">
+      <c r="R8" s="16">
         <v>2015</v>
       </c>
-      <c r="T8" s="17" t="s">
+      <c r="T8" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U8" s="17" t="s">
+      <c r="U8" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V8" s="17" t="s">
+      <c r="V8" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:22">
-      <c r="B9" s="17" t="s">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B9" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C9" s="10"/>
@@ -2409,146 +2412,146 @@
       <c r="P9" s="10"/>
       <c r="Q9" s="10"/>
       <c r="R9" s="10"/>
-      <c r="S9" s="19" t="s">
+      <c r="S9" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T9" s="10"/>
       <c r="U9" s="10"/>
       <c r="V9" s="10"/>
     </row>
-    <row r="13" spans="1:22">
-      <c r="A13" s="16" t="s">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:22">
-      <c r="C14" s="17">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C14" s="16">
         <v>2000</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>2001</v>
       </c>
-      <c r="E14" s="17">
+      <c r="E14" s="16">
         <v>2002</v>
       </c>
-      <c r="F14" s="17">
+      <c r="F14" s="16">
         <v>2003</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="16">
         <v>2004</v>
       </c>
-      <c r="H14" s="17">
+      <c r="H14" s="16">
         <v>2005</v>
       </c>
-      <c r="I14" s="17">
+      <c r="I14" s="16">
         <v>2006</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="16">
         <v>2007</v>
       </c>
-      <c r="K14" s="17">
+      <c r="K14" s="16">
         <v>2008</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="16">
         <v>2009</v>
       </c>
-      <c r="M14" s="17">
+      <c r="M14" s="16">
         <v>2010</v>
       </c>
-      <c r="N14" s="17">
+      <c r="N14" s="16">
         <v>2011</v>
       </c>
-      <c r="O14" s="17">
+      <c r="O14" s="16">
         <v>2012</v>
       </c>
-      <c r="P14" s="17">
+      <c r="P14" s="16">
         <v>2013</v>
       </c>
-      <c r="Q14" s="17">
+      <c r="Q14" s="16">
         <v>2014</v>
       </c>
-      <c r="R14" s="17">
+      <c r="R14" s="16">
         <v>2015</v>
       </c>
-      <c r="T14" s="17" t="s">
+      <c r="T14" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U14" s="17" t="s">
+      <c r="U14" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V14" s="17" t="s">
+      <c r="V14" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:22">
-      <c r="B15" s="17" t="s">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B15" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="17">
         <f t="shared" ref="C15:Q15" si="0">D15/(1.12)</f>
         <v>529043227.23311073</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="17">
         <f t="shared" si="0"/>
         <v>592528414.50108409</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <f t="shared" si="0"/>
         <v>663631824.24121428</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <f t="shared" si="0"/>
         <v>743267643.15016007</v>
       </c>
-      <c r="G15" s="18">
+      <c r="G15" s="17">
         <f t="shared" si="0"/>
         <v>832459760.32817936</v>
       </c>
-      <c r="H15" s="18">
+      <c r="H15" s="17">
         <f t="shared" si="0"/>
         <v>932354931.56756091</v>
       </c>
-      <c r="I15" s="18">
+      <c r="I15" s="17">
         <f t="shared" si="0"/>
         <v>1044237523.3556683</v>
       </c>
-      <c r="J15" s="18">
+      <c r="J15" s="17">
         <f t="shared" si="0"/>
         <v>1169546026.1583486</v>
       </c>
-      <c r="K15" s="18">
+      <c r="K15" s="17">
         <f t="shared" si="0"/>
         <v>1309891549.2973506</v>
       </c>
-      <c r="L15" s="18">
+      <c r="L15" s="17">
         <f t="shared" si="0"/>
         <v>1467078535.213033</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="17">
         <f t="shared" si="0"/>
         <v>1643127959.438597</v>
       </c>
-      <c r="N15" s="18">
+      <c r="N15" s="17">
         <f t="shared" si="0"/>
         <v>1840303314.5712287</v>
       </c>
-      <c r="O15" s="18">
+      <c r="O15" s="17">
         <f t="shared" si="0"/>
         <v>2061139712.3197763</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="17">
         <f t="shared" si="0"/>
         <v>2308476477.7981496</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q15" s="17">
         <f t="shared" si="0"/>
         <v>2585493655.1339278</v>
       </c>
-      <c r="R15" s="18">
+      <c r="R15" s="17">
         <f>3243243241/(1.12)</f>
         <v>2895752893.7499995</v>
       </c>
-      <c r="S15" s="19" t="s">
+      <c r="S15" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T15" s="12">
@@ -2561,138 +2564,138 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="19" spans="1:22">
-      <c r="A19" s="16" t="s">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A19" s="15" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:22">
-      <c r="C20" s="17">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C20" s="16">
         <v>2000</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>2001</v>
       </c>
-      <c r="E20" s="17">
+      <c r="E20" s="16">
         <v>2002</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="16">
         <v>2003</v>
       </c>
-      <c r="G20" s="17">
+      <c r="G20" s="16">
         <v>2004</v>
       </c>
-      <c r="H20" s="17">
+      <c r="H20" s="16">
         <v>2005</v>
       </c>
-      <c r="I20" s="17">
+      <c r="I20" s="16">
         <v>2006</v>
       </c>
-      <c r="J20" s="17">
+      <c r="J20" s="16">
         <v>2007</v>
       </c>
-      <c r="K20" s="17">
+      <c r="K20" s="16">
         <v>2008</v>
       </c>
-      <c r="L20" s="17">
+      <c r="L20" s="16">
         <v>2009</v>
       </c>
-      <c r="M20" s="17">
+      <c r="M20" s="16">
         <v>2010</v>
       </c>
-      <c r="N20" s="17">
+      <c r="N20" s="16">
         <v>2011</v>
       </c>
-      <c r="O20" s="17">
+      <c r="O20" s="16">
         <v>2012</v>
       </c>
-      <c r="P20" s="17">
+      <c r="P20" s="16">
         <v>2013</v>
       </c>
-      <c r="Q20" s="17">
+      <c r="Q20" s="16">
         <v>2014</v>
       </c>
-      <c r="R20" s="17">
+      <c r="R20" s="16">
         <v>2015</v>
       </c>
-      <c r="T20" s="17" t="s">
+      <c r="T20" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U20" s="17" t="s">
+      <c r="U20" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V20" s="17" t="s">
+      <c r="V20" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="1:22">
-      <c r="B21" s="17" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B21" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="19">
         <v>30000000000</v>
       </c>
-      <c r="D21" s="20">
+      <c r="D21" s="19">
         <f>C21+5000000000</f>
         <v>35000000000</v>
       </c>
-      <c r="E21" s="20">
+      <c r="E21" s="19">
         <f t="shared" ref="E21:R21" si="1">D21+5000000000</f>
         <v>40000000000</v>
       </c>
-      <c r="F21" s="20">
+      <c r="F21" s="19">
         <f t="shared" si="1"/>
         <v>45000000000</v>
       </c>
-      <c r="G21" s="20">
+      <c r="G21" s="19">
         <f t="shared" si="1"/>
         <v>50000000000</v>
       </c>
-      <c r="H21" s="20">
+      <c r="H21" s="19">
         <f t="shared" si="1"/>
         <v>55000000000</v>
       </c>
-      <c r="I21" s="20">
+      <c r="I21" s="19">
         <f t="shared" si="1"/>
         <v>60000000000</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="19">
         <f t="shared" si="1"/>
         <v>65000000000</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="19">
         <f t="shared" si="1"/>
         <v>70000000000</v>
       </c>
-      <c r="L21" s="20">
+      <c r="L21" s="19">
         <f t="shared" si="1"/>
         <v>75000000000</v>
       </c>
-      <c r="M21" s="20">
+      <c r="M21" s="19">
         <f t="shared" si="1"/>
         <v>80000000000</v>
       </c>
-      <c r="N21" s="20">
+      <c r="N21" s="19">
         <f t="shared" si="1"/>
         <v>85000000000</v>
       </c>
-      <c r="O21" s="20">
+      <c r="O21" s="19">
         <f t="shared" si="1"/>
         <v>90000000000</v>
       </c>
-      <c r="P21" s="20">
+      <c r="P21" s="19">
         <f t="shared" si="1"/>
         <v>95000000000</v>
       </c>
-      <c r="Q21" s="20">
+      <c r="Q21" s="19">
         <f t="shared" si="1"/>
         <v>100000000000</v>
       </c>
-      <c r="R21" s="20">
+      <c r="R21" s="19">
         <f t="shared" si="1"/>
         <v>105000000000</v>
       </c>
-      <c r="S21" s="19" t="s">
+      <c r="S21" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T21" s="8">
@@ -2705,123 +2708,123 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:22">
-      <c r="A25" s="16" t="s">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A25" s="15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:22">
-      <c r="C26" s="17">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C26" s="16">
         <v>2000</v>
       </c>
-      <c r="D26" s="17">
+      <c r="D26" s="16">
         <v>2001</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="16">
         <v>2002</v>
       </c>
-      <c r="F26" s="17">
+      <c r="F26" s="16">
         <v>2003</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="16">
         <v>2004</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="16">
         <v>2005</v>
       </c>
-      <c r="I26" s="17">
+      <c r="I26" s="16">
         <v>2006</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="16">
         <v>2007</v>
       </c>
-      <c r="K26" s="17">
+      <c r="K26" s="16">
         <v>2008</v>
       </c>
-      <c r="L26" s="17">
+      <c r="L26" s="16">
         <v>2009</v>
       </c>
-      <c r="M26" s="17">
+      <c r="M26" s="16">
         <v>2010</v>
       </c>
-      <c r="N26" s="17">
+      <c r="N26" s="16">
         <v>2011</v>
       </c>
-      <c r="O26" s="17">
+      <c r="O26" s="16">
         <v>2012</v>
       </c>
-      <c r="P26" s="17">
+      <c r="P26" s="16">
         <v>2013</v>
       </c>
-      <c r="Q26" s="17">
+      <c r="Q26" s="16">
         <v>2014</v>
       </c>
-      <c r="R26" s="17">
+      <c r="R26" s="16">
         <v>2015</v>
       </c>
-      <c r="T26" s="17" t="s">
+      <c r="T26" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U26" s="17" t="s">
+      <c r="U26" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V26" s="17" t="s">
+      <c r="V26" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="27" spans="1:22">
-      <c r="B27" s="17" t="s">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B27" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C27" s="21">
+      <c r="C27" s="20">
         <v>30000000000</v>
       </c>
-      <c r="D27" s="21">
+      <c r="D27" s="20">
         <v>35000000000</v>
       </c>
-      <c r="E27" s="21">
+      <c r="E27" s="20">
         <v>40000000000</v>
       </c>
-      <c r="F27" s="21">
+      <c r="F27" s="20">
         <v>45000000000</v>
       </c>
-      <c r="G27" s="21">
+      <c r="G27" s="20">
         <v>50000000000</v>
       </c>
-      <c r="H27" s="21">
+      <c r="H27" s="20">
         <v>55000000000</v>
       </c>
-      <c r="I27" s="21">
+      <c r="I27" s="20">
         <v>60000000000</v>
       </c>
-      <c r="J27" s="21">
+      <c r="J27" s="20">
         <v>65000000000</v>
       </c>
-      <c r="K27" s="21">
+      <c r="K27" s="20">
         <v>70000000000</v>
       </c>
-      <c r="L27" s="21">
+      <c r="L27" s="20">
         <v>75000000000</v>
       </c>
-      <c r="M27" s="21">
+      <c r="M27" s="20">
         <v>80000000000</v>
       </c>
-      <c r="N27" s="21">
+      <c r="N27" s="20">
         <v>85000000000</v>
       </c>
-      <c r="O27" s="21">
+      <c r="O27" s="20">
         <v>90000000000</v>
       </c>
-      <c r="P27" s="21">
+      <c r="P27" s="20">
         <v>95000000000</v>
       </c>
-      <c r="Q27" s="21">
+      <c r="Q27" s="20">
         <v>100000000000</v>
       </c>
-      <c r="R27" s="21">
+      <c r="R27" s="20">
         <v>105000000000</v>
       </c>
-      <c r="S27" s="19" t="s">
+      <c r="S27" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T27" s="12">
@@ -2834,72 +2837,72 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="31" spans="1:22">
-      <c r="A31" s="16" t="s">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A31" s="15" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:22">
-      <c r="C32" s="17">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C32" s="16">
         <v>2000</v>
       </c>
-      <c r="D32" s="17">
+      <c r="D32" s="16">
         <v>2001</v>
       </c>
-      <c r="E32" s="17">
+      <c r="E32" s="16">
         <v>2002</v>
       </c>
-      <c r="F32" s="17">
+      <c r="F32" s="16">
         <v>2003</v>
       </c>
-      <c r="G32" s="17">
+      <c r="G32" s="16">
         <v>2004</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H32" s="16">
         <v>2005</v>
       </c>
-      <c r="I32" s="17">
+      <c r="I32" s="16">
         <v>2006</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="16">
         <v>2007</v>
       </c>
-      <c r="K32" s="17">
+      <c r="K32" s="16">
         <v>2008</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="16">
         <v>2009</v>
       </c>
-      <c r="M32" s="17">
+      <c r="M32" s="16">
         <v>2010</v>
       </c>
-      <c r="N32" s="17">
+      <c r="N32" s="16">
         <v>2011</v>
       </c>
-      <c r="O32" s="17">
+      <c r="O32" s="16">
         <v>2012</v>
       </c>
-      <c r="P32" s="17">
+      <c r="P32" s="16">
         <v>2013</v>
       </c>
-      <c r="Q32" s="17">
+      <c r="Q32" s="16">
         <v>2014</v>
       </c>
-      <c r="R32" s="17">
+      <c r="R32" s="16">
         <v>2015</v>
       </c>
-      <c r="T32" s="17" t="s">
+      <c r="T32" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U32" s="17" t="s">
+      <c r="U32" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V32" s="17" t="s">
+      <c r="V32" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="33" spans="1:22">
-      <c r="B33" s="17" t="s">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B33" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C33" s="10">
@@ -2966,7 +2969,7 @@
         <f t="shared" si="2"/>
         <v>15750000000</v>
       </c>
-      <c r="S33" s="19" t="s">
+      <c r="S33" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T33" s="8">
@@ -2979,139 +2982,139 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:22">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A37" s="15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:22">
-      <c r="C38" s="17">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C38" s="16">
         <v>2000</v>
       </c>
-      <c r="D38" s="17">
+      <c r="D38" s="16">
         <v>2001</v>
       </c>
-      <c r="E38" s="17">
+      <c r="E38" s="16">
         <v>2002</v>
       </c>
-      <c r="F38" s="17">
+      <c r="F38" s="16">
         <v>2003</v>
       </c>
-      <c r="G38" s="17">
+      <c r="G38" s="16">
         <v>2004</v>
       </c>
-      <c r="H38" s="17">
+      <c r="H38" s="16">
         <v>2005</v>
       </c>
-      <c r="I38" s="17">
+      <c r="I38" s="16">
         <v>2006</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="16">
         <v>2007</v>
       </c>
-      <c r="K38" s="17">
+      <c r="K38" s="16">
         <v>2008</v>
       </c>
-      <c r="L38" s="17">
+      <c r="L38" s="16">
         <v>2009</v>
       </c>
-      <c r="M38" s="17">
+      <c r="M38" s="16">
         <v>2010</v>
       </c>
-      <c r="N38" s="17">
+      <c r="N38" s="16">
         <v>2011</v>
       </c>
-      <c r="O38" s="17">
+      <c r="O38" s="16">
         <v>2012</v>
       </c>
-      <c r="P38" s="17">
+      <c r="P38" s="16">
         <v>2013</v>
       </c>
-      <c r="Q38" s="17">
+      <c r="Q38" s="16">
         <v>2014</v>
       </c>
-      <c r="R38" s="17">
+      <c r="R38" s="16">
         <v>2015</v>
       </c>
-      <c r="T38" s="17" t="s">
+      <c r="T38" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U38" s="17" t="s">
+      <c r="U38" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V38" s="17" t="s">
+      <c r="V38" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:22">
-      <c r="B39" s="17" t="s">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B39" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C39" s="18">
+      <c r="C39" s="17">
         <f>12%*C27</f>
         <v>3600000000</v>
       </c>
-      <c r="D39" s="18">
+      <c r="D39" s="17">
         <f t="shared" ref="D39:R39" si="3">12%*D27</f>
         <v>4200000000</v>
       </c>
-      <c r="E39" s="18">
+      <c r="E39" s="17">
         <f t="shared" si="3"/>
         <v>4800000000</v>
       </c>
-      <c r="F39" s="18">
+      <c r="F39" s="17">
         <f t="shared" si="3"/>
         <v>5400000000</v>
       </c>
-      <c r="G39" s="18">
+      <c r="G39" s="17">
         <f t="shared" si="3"/>
         <v>6000000000</v>
       </c>
-      <c r="H39" s="18">
+      <c r="H39" s="17">
         <f t="shared" si="3"/>
         <v>6600000000</v>
       </c>
-      <c r="I39" s="18">
+      <c r="I39" s="17">
         <f t="shared" si="3"/>
         <v>7200000000</v>
       </c>
-      <c r="J39" s="18">
+      <c r="J39" s="17">
         <f t="shared" si="3"/>
         <v>7800000000</v>
       </c>
-      <c r="K39" s="18">
+      <c r="K39" s="17">
         <f t="shared" si="3"/>
         <v>8400000000</v>
       </c>
-      <c r="L39" s="18">
+      <c r="L39" s="17">
         <f t="shared" si="3"/>
         <v>9000000000</v>
       </c>
-      <c r="M39" s="18">
+      <c r="M39" s="17">
         <f t="shared" si="3"/>
         <v>9600000000</v>
       </c>
-      <c r="N39" s="18">
+      <c r="N39" s="17">
         <f t="shared" si="3"/>
         <v>10200000000</v>
       </c>
-      <c r="O39" s="18">
+      <c r="O39" s="17">
         <f t="shared" si="3"/>
         <v>10800000000</v>
       </c>
-      <c r="P39" s="18">
+      <c r="P39" s="17">
         <f t="shared" si="3"/>
         <v>11400000000</v>
       </c>
-      <c r="Q39" s="18">
+      <c r="Q39" s="17">
         <f t="shared" si="3"/>
         <v>12000000000</v>
       </c>
-      <c r="R39" s="18">
+      <c r="R39" s="17">
         <f t="shared" si="3"/>
         <v>12600000000</v>
       </c>
-      <c r="S39" s="19" t="s">
+      <c r="S39" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T39" s="8">
@@ -3124,201 +3127,201 @@
         <v>3.5000000000000003E-2</v>
       </c>
     </row>
-    <row r="43" spans="1:22">
-      <c r="A43" s="16" t="s">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A43" s="15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:22">
-      <c r="C44" s="17">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C44" s="16">
         <v>2000</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="16">
         <v>2001</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="16">
         <v>2002</v>
       </c>
-      <c r="F44" s="17">
+      <c r="F44" s="16">
         <v>2003</v>
       </c>
-      <c r="G44" s="17">
+      <c r="G44" s="16">
         <v>2004</v>
       </c>
-      <c r="H44" s="17">
+      <c r="H44" s="16">
         <v>2005</v>
       </c>
-      <c r="I44" s="17">
+      <c r="I44" s="16">
         <v>2006</v>
       </c>
-      <c r="J44" s="17">
+      <c r="J44" s="16">
         <v>2007</v>
       </c>
-      <c r="K44" s="17">
+      <c r="K44" s="16">
         <v>2008</v>
       </c>
-      <c r="L44" s="17">
+      <c r="L44" s="16">
         <v>2009</v>
       </c>
-      <c r="M44" s="17">
+      <c r="M44" s="16">
         <v>2010</v>
       </c>
-      <c r="N44" s="17">
+      <c r="N44" s="16">
         <v>2011</v>
       </c>
-      <c r="O44" s="17">
+      <c r="O44" s="16">
         <v>2012</v>
       </c>
-      <c r="P44" s="17">
+      <c r="P44" s="16">
         <v>2013</v>
       </c>
-      <c r="Q44" s="17">
+      <c r="Q44" s="16">
         <v>2014</v>
       </c>
-      <c r="R44" s="17">
+      <c r="R44" s="16">
         <v>2015</v>
       </c>
-      <c r="T44" s="17" t="s">
+      <c r="T44" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U44" s="17" t="s">
+      <c r="U44" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V44" s="17" t="s">
+      <c r="V44" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="45" spans="1:22">
-      <c r="B45" s="17" t="s">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B45" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="C45" s="18">
+      <c r="C45" s="17">
         <v>15000000</v>
       </c>
-      <c r="D45" s="18">
+      <c r="D45" s="17">
         <v>16000000</v>
       </c>
-      <c r="E45" s="18">
+      <c r="E45" s="17">
         <v>17000000</v>
       </c>
-      <c r="F45" s="18">
+      <c r="F45" s="17">
         <v>18000000</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="17">
         <v>18000000</v>
       </c>
-      <c r="H45" s="18">
+      <c r="H45" s="17">
         <v>18000000</v>
       </c>
-      <c r="I45" s="18">
+      <c r="I45" s="17">
         <v>18000000</v>
       </c>
-      <c r="J45" s="18">
+      <c r="J45" s="17">
         <v>18000000</v>
       </c>
-      <c r="K45" s="18">
+      <c r="K45" s="17">
         <v>18000000</v>
       </c>
-      <c r="L45" s="18">
+      <c r="L45" s="17">
         <v>18000000</v>
       </c>
-      <c r="M45" s="18">
+      <c r="M45" s="17">
         <v>18000000</v>
       </c>
-      <c r="N45" s="18">
+      <c r="N45" s="17">
         <v>18000000</v>
       </c>
-      <c r="O45" s="18">
+      <c r="O45" s="17">
         <v>18000000</v>
       </c>
-      <c r="P45" s="18">
+      <c r="P45" s="17">
         <v>18000000</v>
       </c>
-      <c r="Q45" s="18">
+      <c r="Q45" s="17">
         <v>18000000</v>
       </c>
-      <c r="R45" s="18">
+      <c r="R45" s="17">
         <v>18000000</v>
       </c>
-      <c r="S45" s="19" t="s">
+      <c r="S45" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="T45" s="22">
+      <c r="T45" s="21">
         <v>0.03</v>
       </c>
-      <c r="U45" s="22">
+      <c r="U45" s="21">
         <v>0.02</v>
       </c>
-      <c r="V45" s="22">
+      <c r="V45" s="21">
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:22">
-      <c r="A49" s="16" t="s">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A49" s="15" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:22">
-      <c r="C50" s="17">
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C50" s="16">
         <v>2000</v>
       </c>
-      <c r="D50" s="17">
+      <c r="D50" s="16">
         <v>2001</v>
       </c>
-      <c r="E50" s="17">
+      <c r="E50" s="16">
         <v>2002</v>
       </c>
-      <c r="F50" s="17">
+      <c r="F50" s="16">
         <v>2003</v>
       </c>
-      <c r="G50" s="17">
+      <c r="G50" s="16">
         <v>2004</v>
       </c>
-      <c r="H50" s="17">
+      <c r="H50" s="16">
         <v>2005</v>
       </c>
-      <c r="I50" s="17">
+      <c r="I50" s="16">
         <v>2006</v>
       </c>
-      <c r="J50" s="17">
+      <c r="J50" s="16">
         <v>2007</v>
       </c>
-      <c r="K50" s="17">
+      <c r="K50" s="16">
         <v>2008</v>
       </c>
-      <c r="L50" s="17">
+      <c r="L50" s="16">
         <v>2009</v>
       </c>
-      <c r="M50" s="17">
+      <c r="M50" s="16">
         <v>2010</v>
       </c>
-      <c r="N50" s="17">
+      <c r="N50" s="16">
         <v>2011</v>
       </c>
-      <c r="O50" s="17">
+      <c r="O50" s="16">
         <v>2012</v>
       </c>
-      <c r="P50" s="17">
+      <c r="P50" s="16">
         <v>2013</v>
       </c>
-      <c r="Q50" s="17">
+      <c r="Q50" s="16">
         <v>2014</v>
       </c>
-      <c r="R50" s="17">
+      <c r="R50" s="16">
         <v>2015</v>
       </c>
-      <c r="T50" s="17" t="s">
+      <c r="T50" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U50" s="17" t="s">
+      <c r="U50" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V50" s="17" t="s">
+      <c r="V50" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:22">
-      <c r="B51" s="17" t="s">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B51" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C51" s="10"/>
@@ -3337,79 +3340,79 @@
       <c r="P51" s="10"/>
       <c r="Q51" s="10"/>
       <c r="R51" s="10"/>
-      <c r="S51" s="19" t="s">
+      <c r="S51" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T51" s="10"/>
       <c r="U51" s="10"/>
       <c r="V51" s="10"/>
     </row>
-    <row r="55" spans="1:22">
-      <c r="A55" s="16" t="s">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A55" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:22">
-      <c r="C56" s="17">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C56" s="16">
         <v>2000</v>
       </c>
-      <c r="D56" s="17">
+      <c r="D56" s="16">
         <v>2001</v>
       </c>
-      <c r="E56" s="17">
+      <c r="E56" s="16">
         <v>2002</v>
       </c>
-      <c r="F56" s="17">
+      <c r="F56" s="16">
         <v>2003</v>
       </c>
-      <c r="G56" s="17">
+      <c r="G56" s="16">
         <v>2004</v>
       </c>
-      <c r="H56" s="17">
+      <c r="H56" s="16">
         <v>2005</v>
       </c>
-      <c r="I56" s="17">
+      <c r="I56" s="16">
         <v>2006</v>
       </c>
-      <c r="J56" s="17">
+      <c r="J56" s="16">
         <v>2007</v>
       </c>
-      <c r="K56" s="17">
+      <c r="K56" s="16">
         <v>2008</v>
       </c>
-      <c r="L56" s="17">
+      <c r="L56" s="16">
         <v>2009</v>
       </c>
-      <c r="M56" s="17">
+      <c r="M56" s="16">
         <v>2010</v>
       </c>
-      <c r="N56" s="17">
+      <c r="N56" s="16">
         <v>2011</v>
       </c>
-      <c r="O56" s="17">
+      <c r="O56" s="16">
         <v>2012</v>
       </c>
-      <c r="P56" s="17">
+      <c r="P56" s="16">
         <v>2013</v>
       </c>
-      <c r="Q56" s="17">
+      <c r="Q56" s="16">
         <v>2014</v>
       </c>
-      <c r="R56" s="17">
+      <c r="R56" s="16">
         <v>2015</v>
       </c>
-      <c r="T56" s="17" t="s">
+      <c r="T56" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U56" s="17" t="s">
+      <c r="U56" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V56" s="17" t="s">
+      <c r="V56" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:22">
-      <c r="B57" s="17" t="s">
+    <row r="57" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B57" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C57" s="10"/>
@@ -3428,79 +3431,79 @@
       <c r="P57" s="10"/>
       <c r="Q57" s="10"/>
       <c r="R57" s="10"/>
-      <c r="S57" s="19" t="s">
+      <c r="S57" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T57" s="10"/>
       <c r="U57" s="10"/>
       <c r="V57" s="10"/>
     </row>
-    <row r="61" spans="1:22">
-      <c r="A61" s="16" t="s">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A61" s="15" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:22">
-      <c r="C62" s="17">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C62" s="16">
         <v>2000</v>
       </c>
-      <c r="D62" s="17">
+      <c r="D62" s="16">
         <v>2001</v>
       </c>
-      <c r="E62" s="17">
+      <c r="E62" s="16">
         <v>2002</v>
       </c>
-      <c r="F62" s="17">
+      <c r="F62" s="16">
         <v>2003</v>
       </c>
-      <c r="G62" s="17">
+      <c r="G62" s="16">
         <v>2004</v>
       </c>
-      <c r="H62" s="17">
+      <c r="H62" s="16">
         <v>2005</v>
       </c>
-      <c r="I62" s="17">
+      <c r="I62" s="16">
         <v>2006</v>
       </c>
-      <c r="J62" s="17">
+      <c r="J62" s="16">
         <v>2007</v>
       </c>
-      <c r="K62" s="17">
+      <c r="K62" s="16">
         <v>2008</v>
       </c>
-      <c r="L62" s="17">
+      <c r="L62" s="16">
         <v>2009</v>
       </c>
-      <c r="M62" s="17">
+      <c r="M62" s="16">
         <v>2010</v>
       </c>
-      <c r="N62" s="17">
+      <c r="N62" s="16">
         <v>2011</v>
       </c>
-      <c r="O62" s="17">
+      <c r="O62" s="16">
         <v>2012</v>
       </c>
-      <c r="P62" s="17">
+      <c r="P62" s="16">
         <v>2013</v>
       </c>
-      <c r="Q62" s="17">
+      <c r="Q62" s="16">
         <v>2014</v>
       </c>
-      <c r="R62" s="17">
+      <c r="R62" s="16">
         <v>2015</v>
       </c>
-      <c r="T62" s="17" t="s">
+      <c r="T62" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U62" s="17" t="s">
+      <c r="U62" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V62" s="17" t="s">
+      <c r="V62" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:22">
-      <c r="B63" s="17" t="s">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B63" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C63" s="10"/>
@@ -3519,79 +3522,79 @@
       <c r="P63" s="10"/>
       <c r="Q63" s="10"/>
       <c r="R63" s="10"/>
-      <c r="S63" s="19" t="s">
+      <c r="S63" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T63" s="10"/>
       <c r="U63" s="10"/>
       <c r="V63" s="10"/>
     </row>
-    <row r="67" spans="1:22">
-      <c r="A67" s="16" t="s">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A67" s="15" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:22">
-      <c r="C68" s="17">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C68" s="16">
         <v>2000</v>
       </c>
-      <c r="D68" s="17">
+      <c r="D68" s="16">
         <v>2001</v>
       </c>
-      <c r="E68" s="17">
+      <c r="E68" s="16">
         <v>2002</v>
       </c>
-      <c r="F68" s="17">
+      <c r="F68" s="16">
         <v>2003</v>
       </c>
-      <c r="G68" s="17">
+      <c r="G68" s="16">
         <v>2004</v>
       </c>
-      <c r="H68" s="17">
+      <c r="H68" s="16">
         <v>2005</v>
       </c>
-      <c r="I68" s="17">
+      <c r="I68" s="16">
         <v>2006</v>
       </c>
-      <c r="J68" s="17">
+      <c r="J68" s="16">
         <v>2007</v>
       </c>
-      <c r="K68" s="17">
+      <c r="K68" s="16">
         <v>2008</v>
       </c>
-      <c r="L68" s="17">
+      <c r="L68" s="16">
         <v>2009</v>
       </c>
-      <c r="M68" s="17">
+      <c r="M68" s="16">
         <v>2010</v>
       </c>
-      <c r="N68" s="17">
+      <c r="N68" s="16">
         <v>2011</v>
       </c>
-      <c r="O68" s="17">
+      <c r="O68" s="16">
         <v>2012</v>
       </c>
-      <c r="P68" s="17">
+      <c r="P68" s="16">
         <v>2013</v>
       </c>
-      <c r="Q68" s="17">
+      <c r="Q68" s="16">
         <v>2014</v>
       </c>
-      <c r="R68" s="17">
+      <c r="R68" s="16">
         <v>2015</v>
       </c>
-      <c r="T68" s="17" t="s">
+      <c r="T68" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U68" s="17" t="s">
+      <c r="U68" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V68" s="17" t="s">
+      <c r="V68" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="69" spans="1:22">
-      <c r="B69" s="17" t="s">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B69" s="16" t="s">
         <v>89</v>
       </c>
       <c r="C69" s="10"/>
@@ -3610,79 +3613,79 @@
       <c r="P69" s="10"/>
       <c r="Q69" s="10"/>
       <c r="R69" s="10"/>
-      <c r="S69" s="19" t="s">
+      <c r="S69" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T69" s="10"/>
       <c r="U69" s="10"/>
       <c r="V69" s="10"/>
     </row>
-    <row r="73" spans="1:22">
-      <c r="A73" s="16" t="s">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A73" s="15" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:22">
-      <c r="C74" s="17">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C74" s="16">
         <v>2000</v>
       </c>
-      <c r="D74" s="17">
+      <c r="D74" s="16">
         <v>2001</v>
       </c>
-      <c r="E74" s="17">
+      <c r="E74" s="16">
         <v>2002</v>
       </c>
-      <c r="F74" s="17">
+      <c r="F74" s="16">
         <v>2003</v>
       </c>
-      <c r="G74" s="17">
+      <c r="G74" s="16">
         <v>2004</v>
       </c>
-      <c r="H74" s="17">
+      <c r="H74" s="16">
         <v>2005</v>
       </c>
-      <c r="I74" s="17">
+      <c r="I74" s="16">
         <v>2006</v>
       </c>
-      <c r="J74" s="17">
+      <c r="J74" s="16">
         <v>2007</v>
       </c>
-      <c r="K74" s="17">
+      <c r="K74" s="16">
         <v>2008</v>
       </c>
-      <c r="L74" s="17">
+      <c r="L74" s="16">
         <v>2009</v>
       </c>
-      <c r="M74" s="17">
+      <c r="M74" s="16">
         <v>2010</v>
       </c>
-      <c r="N74" s="17">
+      <c r="N74" s="16">
         <v>2011</v>
       </c>
-      <c r="O74" s="17">
+      <c r="O74" s="16">
         <v>2012</v>
       </c>
-      <c r="P74" s="17">
+      <c r="P74" s="16">
         <v>2013</v>
       </c>
-      <c r="Q74" s="17">
+      <c r="Q74" s="16">
         <v>2014</v>
       </c>
-      <c r="R74" s="17">
+      <c r="R74" s="16">
         <v>2015</v>
       </c>
-      <c r="T74" s="17" t="s">
+      <c r="T74" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U74" s="17" t="s">
+      <c r="U74" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V74" s="17" t="s">
+      <c r="V74" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="1:22">
-      <c r="B75" s="17" t="s">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B75" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C75" s="11"/>
@@ -3697,13 +3700,13 @@
       <c r="L75" s="11"/>
       <c r="M75" s="11"/>
       <c r="N75" s="11"/>
-      <c r="O75" s="18">
+      <c r="O75" s="17">
         <v>0</v>
       </c>
       <c r="P75" s="11"/>
       <c r="Q75" s="11"/>
       <c r="R75" s="11"/>
-      <c r="S75" s="19" t="s">
+      <c r="S75" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T75" s="8">
@@ -3716,8 +3719,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="76" spans="1:22">
-      <c r="B76" s="17" t="s">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B76" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C76" s="11"/>
@@ -3732,13 +3735,13 @@
       <c r="L76" s="11"/>
       <c r="M76" s="11"/>
       <c r="N76" s="11"/>
-      <c r="O76" s="18">
+      <c r="O76" s="17">
         <v>100</v>
       </c>
       <c r="P76" s="11"/>
       <c r="Q76" s="11"/>
       <c r="R76" s="11"/>
-      <c r="S76" s="19" t="s">
+      <c r="S76" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T76" s="8">
@@ -3751,8 +3754,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="77" spans="1:22">
-      <c r="B77" s="17" t="s">
+    <row r="77" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B77" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C77" s="11"/>
@@ -3767,13 +3770,13 @@
       <c r="L77" s="11"/>
       <c r="M77" s="11"/>
       <c r="N77" s="11"/>
-      <c r="O77" s="18">
+      <c r="O77" s="17">
         <v>100</v>
       </c>
       <c r="P77" s="11"/>
       <c r="Q77" s="11"/>
       <c r="R77" s="11"/>
-      <c r="S77" s="19" t="s">
+      <c r="S77" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T77" s="8">
@@ -3786,8 +3789,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="78" spans="1:22">
-      <c r="B78" s="17" t="s">
+    <row r="78" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B78" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C78" s="11"/>
@@ -3802,13 +3805,13 @@
       <c r="L78" s="11"/>
       <c r="M78" s="11"/>
       <c r="N78" s="11"/>
-      <c r="O78" s="18">
+      <c r="O78" s="17">
         <v>200</v>
       </c>
       <c r="P78" s="11"/>
       <c r="Q78" s="11"/>
       <c r="R78" s="11"/>
-      <c r="S78" s="19" t="s">
+      <c r="S78" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T78" s="8">
@@ -3821,8 +3824,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="79" spans="1:22">
-      <c r="B79" s="17" t="s">
+    <row r="79" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B79" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C79" s="11"/>
@@ -3837,13 +3840,13 @@
       <c r="L79" s="11"/>
       <c r="M79" s="11"/>
       <c r="N79" s="11"/>
-      <c r="O79" s="18">
+      <c r="O79" s="17">
         <v>300</v>
       </c>
       <c r="P79" s="11"/>
       <c r="Q79" s="11"/>
       <c r="R79" s="11"/>
-      <c r="S79" s="19" t="s">
+      <c r="S79" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T79" s="8">
@@ -3856,8 +3859,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="80" spans="1:22">
-      <c r="B80" s="17" t="s">
+    <row r="80" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B80" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C80" s="11"/>
@@ -3872,13 +3875,13 @@
       <c r="L80" s="11"/>
       <c r="M80" s="11"/>
       <c r="N80" s="11"/>
-      <c r="O80" s="18">
+      <c r="O80" s="17">
         <v>500</v>
       </c>
       <c r="P80" s="11"/>
       <c r="Q80" s="11"/>
       <c r="R80" s="11"/>
-      <c r="S80" s="19" t="s">
+      <c r="S80" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T80" s="8">
@@ -3891,72 +3894,72 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="84" spans="1:22">
-      <c r="A84" s="16" t="s">
+    <row r="84" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A84" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="85" spans="1:22">
-      <c r="C85" s="17">
+    <row r="85" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="C85" s="16">
         <v>2000</v>
       </c>
-      <c r="D85" s="17">
+      <c r="D85" s="16">
         <v>2001</v>
       </c>
-      <c r="E85" s="17">
+      <c r="E85" s="16">
         <v>2002</v>
       </c>
-      <c r="F85" s="17">
+      <c r="F85" s="16">
         <v>2003</v>
       </c>
-      <c r="G85" s="17">
+      <c r="G85" s="16">
         <v>2004</v>
       </c>
-      <c r="H85" s="17">
+      <c r="H85" s="16">
         <v>2005</v>
       </c>
-      <c r="I85" s="17">
+      <c r="I85" s="16">
         <v>2006</v>
       </c>
-      <c r="J85" s="17">
+      <c r="J85" s="16">
         <v>2007</v>
       </c>
-      <c r="K85" s="17">
+      <c r="K85" s="16">
         <v>2008</v>
       </c>
-      <c r="L85" s="17">
+      <c r="L85" s="16">
         <v>2009</v>
       </c>
-      <c r="M85" s="17">
+      <c r="M85" s="16">
         <v>2010</v>
       </c>
-      <c r="N85" s="17">
+      <c r="N85" s="16">
         <v>2011</v>
       </c>
-      <c r="O85" s="17">
+      <c r="O85" s="16">
         <v>2012</v>
       </c>
-      <c r="P85" s="17">
+      <c r="P85" s="16">
         <v>2013</v>
       </c>
-      <c r="Q85" s="17">
+      <c r="Q85" s="16">
         <v>2014</v>
       </c>
-      <c r="R85" s="17">
+      <c r="R85" s="16">
         <v>2015</v>
       </c>
-      <c r="T85" s="17" t="s">
+      <c r="T85" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="U85" s="17" t="s">
+      <c r="U85" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="V85" s="17" t="s">
+      <c r="V85" s="16" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="86" spans="1:22">
-      <c r="B86" s="17" t="s">
+    <row r="86" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B86" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C86" s="11"/>
@@ -3977,7 +3980,7 @@
       <c r="P86" s="11"/>
       <c r="Q86" s="11"/>
       <c r="R86" s="11"/>
-      <c r="S86" s="19" t="s">
+      <c r="S86" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T86" s="8">
@@ -3990,8 +3993,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="87" spans="1:22">
-      <c r="B87" s="17" t="s">
+    <row r="87" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B87" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C87" s="11"/>
@@ -4012,7 +4015,7 @@
       <c r="P87" s="11"/>
       <c r="Q87" s="11"/>
       <c r="R87" s="11"/>
-      <c r="S87" s="19" t="s">
+      <c r="S87" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T87" s="8">
@@ -4025,8 +4028,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="88" spans="1:22">
-      <c r="B88" s="17" t="s">
+    <row r="88" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B88" s="16" t="s">
         <v>45</v>
       </c>
       <c r="C88" s="11"/>
@@ -4047,7 +4050,7 @@
       <c r="P88" s="11"/>
       <c r="Q88" s="11"/>
       <c r="R88" s="11"/>
-      <c r="S88" s="19" t="s">
+      <c r="S88" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T88" s="8">
@@ -4060,8 +4063,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="89" spans="1:22">
-      <c r="B89" s="17" t="s">
+    <row r="89" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B89" s="16" t="s">
         <v>28</v>
       </c>
       <c r="C89" s="11"/>
@@ -4082,7 +4085,7 @@
       <c r="P89" s="11"/>
       <c r="Q89" s="11"/>
       <c r="R89" s="11"/>
-      <c r="S89" s="19" t="s">
+      <c r="S89" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T89" s="8">
@@ -4095,8 +4098,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:22">
-      <c r="B90" s="17" t="s">
+    <row r="90" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B90" s="16" t="s">
         <v>29</v>
       </c>
       <c r="C90" s="11"/>
@@ -4117,7 +4120,7 @@
       <c r="P90" s="11"/>
       <c r="Q90" s="11"/>
       <c r="R90" s="11"/>
-      <c r="S90" s="19" t="s">
+      <c r="S90" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T90" s="8">
@@ -4130,8 +4133,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="91" spans="1:22">
-      <c r="B91" s="17" t="s">
+    <row r="91" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B91" s="16" t="s">
         <v>30</v>
       </c>
       <c r="C91" s="11"/>
@@ -4152,7 +4155,7 @@
       <c r="P91" s="11"/>
       <c r="Q91" s="11"/>
       <c r="R91" s="11"/>
-      <c r="S91" s="19" t="s">
+      <c r="S91" s="18" t="s">
         <v>67</v>
       </c>
       <c r="T91" s="8">
@@ -4166,7 +4169,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4178,29 +4180,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="15.75" customWidth="1"/>
-    <col min="4" max="4" width="40.75" customWidth="1"/>
-    <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="8" max="9" width="16.75" customWidth="1"/>
-    <col min="10" max="10" width="12.75" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="40.7109375" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="8" max="9" width="16.7109375" customWidth="1"/>
+    <col min="10" max="10" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="5" t="s">
         <v>135</v>
       </c>
@@ -4229,7 +4231,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="6">
         <v>1</v>
       </c>
@@ -4261,7 +4263,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
         <v>2</v>
       </c>
@@ -4293,12 +4295,12 @@
         <v>147</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C9" s="5" t="s">
         <v>135</v>
       </c>
@@ -4306,7 +4308,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>1</v>
       </c>
@@ -4317,7 +4319,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>2</v>
       </c>
@@ -4329,7 +4331,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4341,7 +4342,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U7"/>
   <sheetViews>
@@ -4349,14 +4350,14 @@
       <selection activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="6">
         <v>2000</v>
       </c>
@@ -4409,7 +4410,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$10</f>
         <v>SBCC</v>
@@ -4448,7 +4449,7 @@
       </c>
       <c r="U3" s="8"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$10</f>
         <v>SBCC</v>
@@ -4487,7 +4488,7 @@
       </c>
       <c r="U4" s="10"/>
     </row>
-    <row r="6" spans="1:21">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="str">
         <f>'Populations &amp; programs'!$C$11</f>
         <v>ART</v>
@@ -4495,42 +4496,42 @@
       <c r="C6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14">
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13"/>
+      <c r="J6" s="13">
         <v>500</v>
       </c>
-      <c r="K6" s="14">
+      <c r="K6" s="13">
         <v>600</v>
       </c>
-      <c r="L6" s="14">
+      <c r="L6" s="13">
         <v>1000</v>
       </c>
-      <c r="M6" s="14">
+      <c r="M6" s="13">
         <v>1200</v>
       </c>
-      <c r="N6" s="14">
+      <c r="N6" s="13">
         <v>1800</v>
       </c>
-      <c r="O6" s="14">
+      <c r="O6" s="13">
         <v>2500</v>
       </c>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14">
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13">
         <v>3000</v>
       </c>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="15" t="s">
+      <c r="R6" s="13"/>
+      <c r="S6" s="13"/>
+      <c r="T6" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="U6" s="14"/>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="U6" s="13"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="str">
         <f>'Populations &amp; programs'!$C$11</f>
         <v>ART</v>
@@ -4574,7 +4575,6 @@
       <c r="U7" s="10"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -4586,7 +4586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:U22"/>
   <sheetViews>
@@ -4594,14 +4594,14 @@
       <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:21">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="6">
         <v>2000</v>
       </c>
@@ -4654,7 +4654,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:21">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -4728,7 +4728,7 @@
       </c>
       <c r="U3" s="10"/>
     </row>
-    <row r="4" spans="1:21">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -4801,7 +4801,7 @@
       </c>
       <c r="U4" s="10"/>
     </row>
-    <row r="5" spans="1:21">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -4875,7 +4875,7 @@
       </c>
       <c r="U5" s="10"/>
     </row>
-    <row r="7" spans="1:21">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -4949,7 +4949,7 @@
       </c>
       <c r="U7" s="10"/>
     </row>
-    <row r="8" spans="1:21">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -5022,7 +5022,7 @@
       </c>
       <c r="U8" s="10"/>
     </row>
-    <row r="9" spans="1:21">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -5096,12 +5096,12 @@
       </c>
       <c r="U9" s="10"/>
     </row>
-    <row r="14" spans="1:21">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:21">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D15" s="6">
         <v>2000</v>
       </c>
@@ -5154,7 +5154,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:21">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -5183,7 +5183,7 @@
       </c>
       <c r="U16" s="8"/>
     </row>
-    <row r="17" spans="2:21">
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -5220,7 +5220,7 @@
       </c>
       <c r="U17" s="8"/>
     </row>
-    <row r="18" spans="2:21">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -5249,7 +5249,7 @@
       </c>
       <c r="U18" s="8"/>
     </row>
-    <row r="20" spans="2:21">
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -5278,7 +5278,7 @@
       </c>
       <c r="U20" s="8"/>
     </row>
-    <row r="21" spans="2:21">
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -5321,7 +5321,7 @@
       </c>
       <c r="U21" s="8"/>
     </row>
-    <row r="22" spans="2:21">
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -5351,7 +5351,6 @@
       <c r="U22" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -5364,20 +5363,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
         <v>2000</v>
       </c>
@@ -5430,7 +5429,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
         <v>89</v>
       </c>
@@ -5455,12 +5454,12 @@
       </c>
       <c r="T3" s="11"/>
     </row>
-    <row r="7" spans="1:20">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C8" s="6">
         <v>2000</v>
       </c>
@@ -5513,7 +5512,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B9" s="6" t="s">
         <v>89</v>
       </c>
@@ -5538,12 +5537,12 @@
       </c>
       <c r="T9" s="11"/>
     </row>
-    <row r="13" spans="1:20">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C14" s="6">
         <v>2000</v>
       </c>
@@ -5596,7 +5595,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B15" s="6" t="s">
         <v>89</v>
       </c>
@@ -5621,12 +5620,12 @@
       </c>
       <c r="T15" s="11"/>
     </row>
-    <row r="19" spans="1:20">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C20" s="6">
         <v>2000</v>
       </c>
@@ -5679,7 +5678,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B21" s="6" t="s">
         <v>89</v>
       </c>
@@ -5704,12 +5703,12 @@
       </c>
       <c r="T21" s="11"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C26" s="6">
         <v>2000</v>
       </c>
@@ -5762,7 +5761,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B27" s="6" t="s">
         <v>89</v>
       </c>
@@ -5787,12 +5786,12 @@
       </c>
       <c r="T27" s="11"/>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C32" s="6">
         <v>2000</v>
       </c>
@@ -5845,7 +5844,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="2:20">
+    <row r="33" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
         <v>89</v>
       </c>
@@ -5871,7 +5870,6 @@
       <c r="T33" s="11"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -5883,7 +5881,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T25"/>
   <sheetViews>
@@ -5891,14 +5889,14 @@
       <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
         <v>2000</v>
       </c>
@@ -5951,7 +5949,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -5979,7 +5977,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6007,12 +6005,12 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>2000</v>
       </c>
@@ -6065,7 +6063,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -6097,7 +6095,7 @@
       </c>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6131,12 +6129,12 @@
       </c>
       <c r="T11" s="8"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="6">
         <v>2000</v>
       </c>
@@ -6189,7 +6187,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -6217,7 +6215,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6249,12 +6247,12 @@
       </c>
       <c r="T18" s="8"/>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23" s="6">
         <v>2000</v>
       </c>
@@ -6307,7 +6305,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -6335,7 +6333,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6364,7 +6362,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -6376,22 +6373,20 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J22" workbookViewId="0">
-      <selection activeCell="T48" sqref="T48"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
         <v>2000</v>
       </c>
@@ -6444,7 +6439,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -6472,7 +6467,7 @@
       </c>
       <c r="T3" s="12"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6500,12 +6495,12 @@
       </c>
       <c r="T4" s="12"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>2000</v>
       </c>
@@ -6558,7 +6553,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
         <v>101</v>
       </c>
@@ -6585,12 +6580,12 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:20">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C15" s="6">
         <v>2000</v>
       </c>
@@ -6643,56 +6638,56 @@
         <v>79</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="13"/>
+      <c r="I16" s="13">
         <f>'Cost &amp; coverage'!J6</f>
         <v>500</v>
       </c>
-      <c r="J16" s="14">
+      <c r="J16" s="13">
         <f>'Cost &amp; coverage'!K6</f>
         <v>600</v>
       </c>
-      <c r="K16" s="14">
+      <c r="K16" s="13">
         <f>'Cost &amp; coverage'!L6</f>
         <v>1000</v>
       </c>
-      <c r="L16" s="14">
+      <c r="L16" s="13">
         <f>'Cost &amp; coverage'!M6</f>
         <v>1200</v>
       </c>
-      <c r="M16" s="14">
+      <c r="M16" s="13">
         <f>'Cost &amp; coverage'!N6</f>
         <v>1800</v>
       </c>
-      <c r="N16" s="14">
+      <c r="N16" s="13">
         <v>2000</v>
       </c>
-      <c r="O16" s="14"/>
-      <c r="P16" s="14">
+      <c r="O16" s="13"/>
+      <c r="P16" s="13">
         <v>2400</v>
       </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
       <c r="S16" s="9" t="s">
         <v>81</v>
       </c>
       <c r="T16" s="7"/>
     </row>
-    <row r="20" spans="1:20">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="1:20">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C21" s="6">
         <v>2000</v>
       </c>
@@ -6745,7 +6740,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B22" s="6" t="s">
         <v>89</v>
       </c>
@@ -6774,12 +6769,12 @@
       </c>
       <c r="T22" s="7"/>
     </row>
-    <row r="26" spans="1:20">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="27" spans="1:20">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C27" s="6">
         <v>2000</v>
       </c>
@@ -6832,7 +6827,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:20">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B28" s="6" t="s">
         <v>89</v>
       </c>
@@ -6877,12 +6872,12 @@
       </c>
       <c r="T28" s="7"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="33" spans="1:20">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C33" s="6">
         <v>2000</v>
       </c>
@@ -6935,7 +6930,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:20">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B34" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -6961,7 +6956,7 @@
       </c>
       <c r="T34" s="12"/>
     </row>
-    <row r="35" spans="1:20">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B35" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -6989,12 +6984,12 @@
       </c>
       <c r="T35" s="12"/>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:20">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C40" s="6">
         <v>2000</v>
       </c>
@@ -7047,7 +7042,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="41" spans="1:20">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>89</v>
       </c>
@@ -7078,12 +7073,12 @@
       </c>
       <c r="T41" s="7"/>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:20">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C46" s="6">
         <v>2000</v>
       </c>
@@ -7136,7 +7131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="47" spans="1:20">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7164,12 +7159,12 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="51" spans="1:20">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="52" spans="1:20">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C52" s="6">
         <v>2000</v>
       </c>
@@ -7222,7 +7217,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="53" spans="1:20">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B53" s="6" t="s">
         <v>89</v>
       </c>
@@ -7250,7 +7245,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -7263,22 +7257,22 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T45"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
         <v>2000</v>
       </c>
@@ -7331,7 +7325,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7342,17 +7336,17 @@
       <c r="F3" s="7"/>
       <c r="G3" s="7"/>
       <c r="H3" s="7">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="I3" s="7"/>
       <c r="J3" s="7"/>
       <c r="K3" s="7">
-        <v>55</v>
+        <v>120</v>
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
       <c r="N3" s="7">
-        <v>54</v>
+        <v>184</v>
       </c>
       <c r="O3" s="7"/>
       <c r="P3" s="7"/>
@@ -7363,7 +7357,7 @@
       </c>
       <c r="T3" s="7"/>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7374,17 +7368,17 @@
       <c r="F4" s="7"/>
       <c r="G4" s="7"/>
       <c r="H4" s="7">
-        <v>40</v>
+        <v>113</v>
       </c>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7">
-        <v>45</v>
+        <v>124</v>
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7">
-        <v>53</v>
+        <v>136</v>
       </c>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
@@ -7395,12 +7389,12 @@
       </c>
       <c r="T4" s="7"/>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>2000</v>
       </c>
@@ -7453,7 +7447,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7481,7 +7475,7 @@
       </c>
       <c r="T10" s="7"/>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7509,12 +7503,12 @@
       </c>
       <c r="T11" s="7"/>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="6">
         <v>2000</v>
       </c>
@@ -7567,7 +7561,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="1:20">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7595,7 +7589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B18" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7623,12 +7617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:20">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="23" spans="1:20">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C23" s="6">
         <v>2000</v>
       </c>
@@ -7681,7 +7675,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="24" spans="1:20">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B24" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7713,7 +7707,7 @@
       </c>
       <c r="T24" s="12"/>
     </row>
-    <row r="25" spans="1:20">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B25" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7743,12 +7737,12 @@
       </c>
       <c r="T25" s="12"/>
     </row>
-    <row r="29" spans="1:20">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="30" spans="1:20">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C30" s="6">
         <v>2000</v>
       </c>
@@ -7801,7 +7795,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="31" spans="1:20">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B31" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7829,7 +7823,7 @@
       </c>
       <c r="T31" s="12"/>
     </row>
-    <row r="32" spans="1:20">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7857,12 +7851,12 @@
       </c>
       <c r="T32" s="12"/>
     </row>
-    <row r="36" spans="1:20">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:20">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C37" s="6">
         <v>2000</v>
       </c>
@@ -7915,7 +7909,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:20">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -7943,7 +7937,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -7971,12 +7965,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="44" spans="1:20">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C44" s="6">
         <v>2000</v>
       </c>
@@ -8029,7 +8023,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:20">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -8058,7 +8052,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -8070,7 +8063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:T17"/>
   <sheetViews>
@@ -8078,14 +8071,14 @@
       <selection activeCell="T18" sqref="T18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:20">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C2" s="6">
         <v>2000</v>
       </c>
@@ -8138,7 +8131,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -8166,7 +8159,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -8194,12 +8187,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:20">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="9" spans="1:20">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>2000</v>
       </c>
@@ -8252,7 +8245,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="10" spans="1:20">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="str">
         <f>'Populations &amp; programs'!$C$3</f>
         <v>Males 15-49</v>
@@ -8280,7 +8273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:20">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" s="6" t="str">
         <f>'Populations &amp; programs'!$C$4</f>
         <v>Females 15-49</v>
@@ -8308,12 +8301,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:20">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="6">
         <v>2000</v>
       </c>
@@ -8366,7 +8359,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="17" spans="2:20">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" s="6" t="s">
         <v>101</v>
       </c>
@@ -8394,7 +8387,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>